<commit_message>
beresin lampiran rks barang tunjuk langsung
</commit_message>
<xml_diff>
--- a/templates/PL-B-Lamp_3.xlsx
+++ b/templates/PL-B-Lamp_3.xlsx
@@ -222,15 +222,12 @@
       <charset val="238"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGray"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -427,46 +424,23 @@
       <alignment horizontal="centerContinuous"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -481,6 +455,29 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -854,9 +851,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C1:I92"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6:H6"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
@@ -868,176 +863,176 @@
   </cols>
   <sheetData>
     <row r="1" spans="3:9" ht="18.75">
-      <c r="D1" s="32" t="s">
+      <c r="D1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="35" t="s">
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="26" t="s">
         <v>1</v>
       </c>
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="3:9" ht="14.25">
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
       <c r="I2" s="2"/>
     </row>
     <row r="3" spans="3:9" ht="15.75">
-      <c r="C3" s="38" t="s">
+      <c r="C3" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="30"/>
       <c r="I3" s="2"/>
     </row>
     <row r="4" spans="3:9" ht="15.75">
-      <c r="C4" s="38" t="s">
+      <c r="C4" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="D4" s="39"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="39"/>
-      <c r="H4" s="39"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
       <c r="I4" s="2"/>
     </row>
     <row r="5" spans="3:9" ht="15.75">
-      <c r="C5" s="40" t="s">
+      <c r="C5" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="D5" s="39"/>
-      <c r="E5" s="39"/>
-      <c r="F5" s="39"/>
-      <c r="G5" s="39"/>
-      <c r="H5" s="39"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="30"/>
       <c r="I5" s="2"/>
     </row>
     <row r="6" spans="3:9" ht="14.25">
-      <c r="C6" s="36" t="s">
+      <c r="C6" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="D6" s="39"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
-      <c r="G6" s="39"/>
-      <c r="H6" s="39"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="30"/>
       <c r="I6" s="2"/>
     </row>
     <row r="7" spans="3:9" ht="14.25">
-      <c r="C7" s="36" t="s">
+      <c r="C7" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="D7" s="37"/>
-      <c r="E7" s="37"/>
-      <c r="F7" s="37"/>
-      <c r="G7" s="37"/>
-      <c r="H7" s="37"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="28"/>
       <c r="I7" s="2"/>
     </row>
     <row r="8" spans="3:9" ht="14.25">
-      <c r="C8" s="36" t="s">
+      <c r="C8" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="D8" s="37"/>
-      <c r="E8" s="37"/>
-      <c r="F8" s="37"/>
-      <c r="G8" s="37"/>
-      <c r="H8" s="37"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="28"/>
       <c r="I8" s="2"/>
     </row>
     <row r="9" spans="3:9" ht="15" thickBot="1">
-      <c r="C9" s="27"/>
-      <c r="D9" s="27"/>
-      <c r="E9" s="27"/>
-      <c r="F9" s="27"/>
-      <c r="G9" s="27"/>
-      <c r="H9" s="27"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="19"/>
       <c r="I9" s="2"/>
     </row>
     <row r="10" spans="3:9" ht="16.5" thickTop="1" thickBot="1">
-      <c r="C10" s="19"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="29"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="20" t="s">
+      <c r="C10" s="32"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="33"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="H10" s="21"/>
+      <c r="H10" s="35"/>
       <c r="I10" s="2"/>
     </row>
     <row r="11" spans="3:9" ht="15">
-      <c r="C11" s="22" t="s">
+      <c r="C11" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="D11" s="22" t="s">
+      <c r="D11" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="E11" s="22" t="s">
+      <c r="E11" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="F11" s="22" t="s">
+      <c r="F11" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="G11" s="22" t="s">
+      <c r="G11" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="H11" s="23" t="s">
+      <c r="H11" s="37" t="s">
         <v>9</v>
       </c>
       <c r="I11" s="2"/>
     </row>
     <row r="12" spans="3:9" ht="15.75" thickBot="1">
-      <c r="C12" s="24"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="25" t="s">
+      <c r="C12" s="38"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="F12" s="24"/>
-      <c r="G12" s="25" t="s">
+      <c r="F12" s="38"/>
+      <c r="G12" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="H12" s="26" t="s">
+      <c r="H12" s="40" t="s">
         <v>11</v>
       </c>
       <c r="I12" s="2"/>
     </row>
     <row r="13" spans="3:9" ht="15.75" thickBot="1">
-      <c r="C13" s="25">
+      <c r="C13" s="39">
         <v>1</v>
       </c>
-      <c r="D13" s="25">
+      <c r="D13" s="39">
         <v>2</v>
       </c>
-      <c r="E13" s="25">
+      <c r="E13" s="39">
         <v>3</v>
       </c>
-      <c r="F13" s="25">
+      <c r="F13" s="39">
         <v>4</v>
       </c>
-      <c r="G13" s="25">
+      <c r="G13" s="39">
         <v>5</v>
       </c>
-      <c r="H13" s="26">
+      <c r="H13" s="40">
         <v>6</v>
       </c>
       <c r="I13" s="2"/>
     </row>
     <row r="14" spans="3:9" ht="15">
-      <c r="C14" s="33"/>
-      <c r="D14" s="33"/>
-      <c r="E14" s="33"/>
-      <c r="F14" s="33"/>
-      <c r="G14" s="33"/>
-      <c r="H14" s="34"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="25"/>
       <c r="I14" s="2"/>
     </row>
     <row r="15" spans="3:9" ht="15">
@@ -1055,10 +1050,10 @@
     </row>
     <row r="16" spans="3:9" ht="15">
       <c r="C16" s="7"/>
-      <c r="D16" s="28" t="s">
+      <c r="D16" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="E16" s="28"/>
+      <c r="E16" s="20"/>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
       <c r="H16" s="5"/>
@@ -1121,7 +1116,7 @@
     </row>
     <row r="22" spans="3:9" ht="15.75" thickBot="1">
       <c r="C22" s="7"/>
-      <c r="D22" s="30" t="s">
+      <c r="D22" s="21" t="s">
         <v>20</v>
       </c>
       <c r="E22" s="3"/>
@@ -1222,7 +1217,7 @@
     </row>
     <row r="31" spans="3:9" ht="15.75" thickBot="1">
       <c r="C31" s="7"/>
-      <c r="D31" s="30" t="s">
+      <c r="D31" s="21" t="s">
         <v>24</v>
       </c>
       <c r="E31" s="3"/>
@@ -1279,7 +1274,7 @@
     </row>
     <row r="36" spans="3:9" ht="15">
       <c r="C36" s="7"/>
-      <c r="D36" s="30" t="s">
+      <c r="D36" s="21" t="s">
         <v>27</v>
       </c>
       <c r="E36" s="3"/>
@@ -1325,7 +1320,7 @@
     </row>
     <row r="40" spans="3:9" ht="15.75" thickBot="1">
       <c r="C40" s="8"/>
-      <c r="D40" s="31" t="s">
+      <c r="D40" s="22" t="s">
         <v>30</v>
       </c>
       <c r="E40" s="1"/>

</xml_diff>